<commit_message>
final update on paragrading
</commit_message>
<xml_diff>
--- a/para_grading/ML/Tests/CompTime.xlsx
+++ b/para_grading/ML/Tests/CompTime.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Stemming</t>
   </si>
@@ -46,6 +46,57 @@
   </si>
   <si>
     <t>Trouble (7)</t>
+  </si>
+  <si>
+    <t>Sem_internal_word_WSD</t>
+  </si>
+  <si>
+    <t>Sem_internal_sentence_WSD</t>
+  </si>
+  <si>
+    <t>Sem_corpus_word_WSD</t>
+  </si>
+  <si>
+    <t>Sem_corpus_sentence_WSD</t>
+  </si>
+  <si>
+    <t>Term extraction (topia)</t>
+  </si>
+  <si>
+    <t>Negation ngram construction</t>
+  </si>
+  <si>
+    <t>WUP</t>
+  </si>
+  <si>
+    <t>JNC</t>
+  </si>
+  <si>
+    <t>Sem_corpus_sentence_WSD_JNC</t>
+  </si>
+  <si>
+    <t>CommEng</t>
+  </si>
+  <si>
+    <t>SelfDefine</t>
+  </si>
+  <si>
+    <t>0.078-0.016</t>
+  </si>
+  <si>
+    <t>0.047-0.016</t>
+  </si>
+  <si>
+    <t>bigram</t>
+  </si>
+  <si>
+    <t>trigram</t>
+  </si>
+  <si>
+    <t>Threshold</t>
+  </si>
+  <si>
+    <t>POS + Neg Bi</t>
   </si>
 </sst>
 </file>
@@ -377,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -399,102 +450,258 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>7.1999999999999995E-2</v>
-      </c>
-      <c r="C2">
-        <v>3.5999999999999997E-2</v>
-      </c>
-      <c r="D2">
-        <v>1.6E-2</v>
-      </c>
-    </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="B3">
-        <v>2.5470000000000002</v>
-      </c>
-      <c r="C3">
-        <v>2.5710000000000002</v>
-      </c>
-      <c r="D3">
-        <v>2.496</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="B4">
-        <v>12.439</v>
-      </c>
-      <c r="C4">
-        <v>11.289</v>
-      </c>
-      <c r="D4">
-        <v>9.2200000000000006</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6">
-        <v>10.211</v>
-      </c>
-      <c r="C6">
-        <v>8.4480000000000004</v>
-      </c>
-      <c r="D6">
-        <v>6.4580000000000002</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7">
-        <v>10.257999999999999</v>
-      </c>
-      <c r="C7">
-        <v>8.859</v>
-      </c>
-      <c r="D7">
-        <v>6.49</v>
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8">
-        <v>10.089</v>
-      </c>
-      <c r="C8">
-        <v>7.9740000000000002</v>
-      </c>
-      <c r="D8">
-        <v>6.5519999999999996</v>
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="C10">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="D10">
+        <v>1.6E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>2.5470000000000002</v>
+      </c>
+      <c r="C11">
+        <v>2.5710000000000002</v>
+      </c>
+      <c r="D11">
+        <v>2.496</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>12.439</v>
+      </c>
+      <c r="C12">
+        <v>11.289</v>
+      </c>
+      <c r="D12">
+        <v>9.2200000000000006</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14">
+        <v>10.099</v>
+      </c>
+      <c r="C14">
+        <v>8.2680000000000007</v>
+      </c>
+      <c r="D14">
+        <v>6.6219999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15">
+        <v>10.211</v>
+      </c>
+      <c r="C15">
+        <v>8.4480000000000004</v>
+      </c>
+      <c r="D15">
+        <v>6.4580000000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>0.30199999999999999</v>
+      </c>
+      <c r="C16">
+        <v>0.26700000000000002</v>
+      </c>
+      <c r="D16">
+        <v>0.25600000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18">
+        <v>10.257999999999999</v>
+      </c>
+      <c r="C18">
+        <v>8.859</v>
+      </c>
+      <c r="D18">
+        <v>6.49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19">
+        <v>10.089</v>
+      </c>
+      <c r="C19">
+        <v>7.9740000000000002</v>
+      </c>
+      <c r="D19">
+        <v>6.5519999999999996</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
         <v>6</v>
       </c>
-      <c r="B10">
+      <c r="B21">
         <v>4.6239999999999997</v>
       </c>
-      <c r="C10">
+      <c r="C21">
         <v>2.8540000000000001</v>
       </c>
-      <c r="D10">
+      <c r="D21">
         <v>2.589</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22">
+        <v>139.85400000000001</v>
+      </c>
+      <c r="C22">
+        <v>61.790999999999997</v>
+      </c>
+      <c r="D22">
+        <v>19.905000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23">
+        <v>136.4</v>
+      </c>
+      <c r="C23">
+        <v>61.058</v>
+      </c>
+      <c r="D23">
+        <v>20.013999999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24">
+        <v>1721.1569999999999</v>
+      </c>
+      <c r="C24">
+        <v>481.46899999999999</v>
+      </c>
+      <c r="D24">
+        <v>49.750999999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25">
+        <v>1723.1030000000001</v>
+      </c>
+      <c r="C25">
+        <v>486.50700000000001</v>
+      </c>
+      <c r="D25">
+        <v>50.783999999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" t="s">
+        <v>16</v>
+      </c>
+      <c r="B27">
+        <v>162.56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28">
+        <v>554.69200000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30">
+        <v>730.32899999999995</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" t="s">
+        <v>26</v>
+      </c>
+      <c r="B32">
+        <v>9.875</v>
       </c>
     </row>
   </sheetData>

</xml_diff>